<commit_message>
subject added on Tuesday by yann
</commit_message>
<xml_diff>
--- a/Mappe11.xlsx
+++ b/Mappe11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Master\Sommer\WPM-Advanced Programing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CA8D16D-0369-4FC2-B96A-4CCF228C8CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA9A9E9-75AF-4ECB-A3F8-E8951AD86BF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FB3ADDF8-02BC-4528-A921-B476326FB9AE}"/>
+    <workbookView xWindow="39570" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB3ADDF8-02BC-4528-A921-B476326FB9AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>lundi</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>22h-23h</t>
+  </si>
+  <si>
+    <t>Mustererkennung(yann)</t>
   </si>
 </sst>
 </file>
@@ -495,14 +498,16 @@
   <dimension ref="D3:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="11" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,7 +567,9 @@
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="4:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">

</xml_diff>